<commit_message>
add addressing + final programm
</commit_message>
<xml_diff>
--- a/controls.xlsx
+++ b/controls.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="COMMANDS" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="230">
   <si>
     <t>#</t>
   </si>
@@ -356,9 +356,6 @@
     <t>00001100</t>
   </si>
   <si>
-    <t>DIRECT</t>
-  </si>
-  <si>
     <t>IR2 -&gt; AR</t>
   </si>
   <si>
@@ -398,9 +395,6 @@
     <t>10, 27, 28</t>
   </si>
   <si>
-    <t>RELATIVE</t>
-  </si>
-  <si>
     <t>DR -&gt; AR</t>
   </si>
   <si>
@@ -497,9 +491,6 @@
     <t>10, 20, 19, 50, 51, 52</t>
   </si>
   <si>
-    <t>00010100</t>
-  </si>
-  <si>
     <t>AR out, MEM en</t>
   </si>
   <si>
@@ -693,6 +684,42 @@
   </si>
   <si>
     <t>00011000</t>
+  </si>
+  <si>
+    <t>RELATIVEx2</t>
+  </si>
+  <si>
+    <t>Relative</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>IR2 -&gt; OP1</t>
+  </si>
+  <si>
+    <t>IR3 -&gt; OP2</t>
+  </si>
+  <si>
+    <t>IR2_ENABLE,  OP1_ENABLE, OP1_RW</t>
+  </si>
+  <si>
+    <t>IR3_ENABLE, OP2_ENABLE, OP2_RW</t>
+  </si>
+  <si>
+    <t>3, 27, 28</t>
+  </si>
+  <si>
+    <t>5, 29, 30</t>
+  </si>
+  <si>
+    <t>Косвенная косвенная</t>
+  </si>
+  <si>
+    <t>Косвенная x2</t>
+  </si>
+  <si>
+    <t>00010110</t>
   </si>
 </sst>
 </file>
@@ -787,7 +814,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="715">
+  <cellStyleXfs count="725">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1503,8 +1530,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1559,6 +1596,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1575,8 +1615,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="715">
+  <cellStyles count="725">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1934,6 +1980,11 @@
     <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2291,6 +2342,11 @@
     <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2590,10 +2646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2626,22 +2682,22 @@
         <v>75</v>
       </c>
       <c r="F1" s="20"/>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="30" t="s">
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="11">
@@ -2670,9 +2726,9 @@
       <c r="J2" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
       <c r="N2" s="10"/>
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
@@ -2762,7 +2818,7 @@
         <v>6</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L4" s="16" t="str">
         <f t="shared" ref="L4:L18" si="2">DEC2BIN(I4,8)</f>
@@ -2808,7 +2864,7 @@
         <v>70</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>78</v>
+        <v>228</v>
       </c>
       <c r="I5" s="11">
         <v>12</v>
@@ -2817,7 +2873,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>155</v>
+        <v>229</v>
       </c>
       <c r="L5" s="16" t="str">
         <f t="shared" si="2"/>
@@ -2829,7 +2885,7 @@
       </c>
       <c r="N5" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>0014</v>
+        <v>0016</v>
       </c>
       <c r="O5" s="11" t="str">
         <f t="shared" si="5"/>
@@ -2860,7 +2916,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>78</v>
@@ -2872,7 +2928,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="L6" s="16" t="str">
         <f t="shared" si="2"/>
@@ -2915,7 +2971,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>77</v>
@@ -2927,7 +2983,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="L7" s="16" t="str">
         <f t="shared" si="2"/>
@@ -2956,7 +3012,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C8" s="12">
         <v>1</v>
@@ -2970,7 +3026,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>78</v>
@@ -2982,7 +3038,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L8" s="16" t="str">
         <f t="shared" si="2"/>
@@ -3011,7 +3067,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C9" s="11">
         <v>1</v>
@@ -3025,7 +3081,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>78</v>
@@ -3037,7 +3093,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="L9" s="16" t="str">
         <f t="shared" si="2"/>
@@ -3080,7 +3136,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>78</v>
@@ -3092,7 +3148,7 @@
         <v>33</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L10" s="16" t="str">
         <f t="shared" si="2"/>
@@ -3121,7 +3177,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C11" s="12">
         <v>1</v>
@@ -3135,7 +3191,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>78</v>
@@ -3147,7 +3203,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="L11" s="16" t="str">
         <f t="shared" si="2"/>
@@ -3176,7 +3232,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C12" s="12">
         <v>1</v>
@@ -3432,11 +3488,11 @@
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10" t="s">
+      <c r="A19" s="25"/>
+      <c r="B19" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="25" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3445,7 +3501,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C20" s="15">
         <v>0</v>
@@ -3456,106 +3512,132 @@
         <v>2</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C21" s="15">
         <v>1</v>
       </c>
     </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="11">
+        <v>3</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C22" s="11">
+        <v>2</v>
+      </c>
+    </row>
     <row r="23" spans="1:16" ht="16">
-      <c r="A23" s="11"/>
+      <c r="A23" s="11">
+        <v>4</v>
+      </c>
       <c r="B23" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>183</v>
+        <v>78</v>
+      </c>
+      <c r="C23" s="11">
+        <v>3</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:16" ht="16">
-      <c r="A24" s="11">
-        <v>1</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="C24" s="11">
-        <v>2</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>184</v>
-      </c>
       <c r="G24" s="23"/>
       <c r="H24" s="3"/>
       <c r="J24" s="18"/>
     </row>
     <row r="25" spans="1:16" ht="16">
-      <c r="A25" s="11">
-        <v>2</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="C25" s="11">
-        <v>2</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>185</v>
-      </c>
       <c r="G25" s="23"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:16" ht="16">
-      <c r="A26" s="11">
-        <v>3</v>
-      </c>
+      <c r="A26" s="11"/>
       <c r="B26" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="D26" s="24" t="s">
         <v>180</v>
-      </c>
-      <c r="C26" s="11">
-        <v>2</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>186</v>
       </c>
       <c r="G26" s="23"/>
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:16" ht="16">
       <c r="A27" s="11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B27" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" s="11">
+        <v>2</v>
+      </c>
+      <c r="D27" s="24" t="s">
         <v>181</v>
-      </c>
-      <c r="C27" s="11">
-        <v>1</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>187</v>
       </c>
       <c r="G27" s="23"/>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:16" ht="16">
       <c r="A28" s="11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B28" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C28" s="11">
+        <v>2</v>
+      </c>
+      <c r="D28" s="24" t="s">
         <v>182</v>
-      </c>
-      <c r="C28" s="11">
-        <v>1</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>188</v>
       </c>
       <c r="G28" s="23"/>
       <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="11">
+        <v>3</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C29" s="11">
+        <v>2</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="11">
+        <v>4</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C30" s="11">
+        <v>1</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="11">
+        <v>5</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" s="11">
+        <v>1</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>185</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3595,7 +3677,7 @@
   <sheetData>
     <row r="1" spans="1:68">
       <c r="A1" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>44</v>
@@ -3606,72 +3688,72 @@
       <c r="D1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="31"/>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="31"/>
-      <c r="BH1" s="31"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="31"/>
-      <c r="BM1" s="31"/>
-      <c r="BN1" s="31"/>
-      <c r="BO1" s="31"/>
-      <c r="BP1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="32"/>
+      <c r="BH1" s="32"/>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BM1" s="32"/>
+      <c r="BN1" s="32"/>
+      <c r="BO1" s="32"/>
+      <c r="BP1" s="32"/>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="10" t="s">
@@ -3685,13 +3767,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:68">
@@ -3700,13 +3782,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:68">
@@ -3715,10 +3797,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>88</v>
@@ -3729,13 +3811,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:68">
@@ -3743,13 +3825,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:68">
@@ -3757,13 +3839,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:68">
@@ -3777,19 +3859,19 @@
         <v>25</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:68">
       <c r="B11" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3811,7 +3893,7 @@
   <dimension ref="A1:BP27"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3827,7 +3909,7 @@
   <sheetData>
     <row r="1" spans="1:68">
       <c r="A1" s="11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>44</v>
@@ -3838,72 +3920,72 @@
       <c r="D1" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="31"/>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="31"/>
-      <c r="BH1" s="31"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="31"/>
-      <c r="BM1" s="31"/>
-      <c r="BN1" s="31"/>
-      <c r="BO1" s="31"/>
-      <c r="BP1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="32"/>
+      <c r="BH1" s="32"/>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BM1" s="32"/>
+      <c r="BN1" s="32"/>
+      <c r="BO1" s="32"/>
+      <c r="BP1" s="32"/>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="25" t="s">
@@ -3918,13 +4000,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:68">
@@ -3933,13 +4015,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:68">
@@ -3948,10 +4030,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>88</v>
@@ -3962,13 +4044,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:68">
@@ -3976,13 +4058,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:68">
@@ -3990,13 +4072,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:68">
@@ -4004,10 +4086,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>88</v>
@@ -4019,13 +4101,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:68">
@@ -4034,13 +4116,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:68">
@@ -4049,13 +4131,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:68">
@@ -4064,13 +4146,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:68">
@@ -4085,19 +4167,19 @@
         <v>25</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:68">
       <c r="B16" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4146,72 +4228,72 @@
       <c r="E1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="31"/>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="31"/>
-      <c r="BH1" s="31"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="31"/>
-      <c r="BM1" s="31"/>
-      <c r="BN1" s="31"/>
-      <c r="BO1" s="31"/>
-      <c r="BP1" s="31"/>
-      <c r="BQ1" s="31"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="32"/>
+      <c r="BH1" s="32"/>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BM1" s="32"/>
+      <c r="BN1" s="32"/>
+      <c r="BO1" s="32"/>
+      <c r="BP1" s="32"/>
+      <c r="BQ1" s="32"/>
     </row>
     <row r="2" spans="1:69">
       <c r="A2" s="10" t="s">
@@ -4292,11 +4374,11 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4316,8 +4398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D234"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4620,7 +4702,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4943,681 +5025,681 @@
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="26"/>
-      <c r="B66" s="27"/>
-      <c r="C66" s="27"/>
+      <c r="A66" s="27"/>
+      <c r="B66" s="28"/>
+      <c r="C66" s="28"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="26"/>
-      <c r="B67" s="27"/>
+      <c r="A67" s="27"/>
+      <c r="B67" s="28"/>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="26"/>
-      <c r="B68" s="27"/>
+      <c r="A68" s="27"/>
+      <c r="B68" s="28"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="26"/>
-      <c r="B69" s="27"/>
+      <c r="A69" s="27"/>
+      <c r="B69" s="28"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="26"/>
-      <c r="B70" s="27"/>
+      <c r="A70" s="27"/>
+      <c r="B70" s="28"/>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="26"/>
-      <c r="B71" s="27"/>
+      <c r="A71" s="27"/>
+      <c r="B71" s="28"/>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="26"/>
-      <c r="B72" s="27"/>
+      <c r="A72" s="27"/>
+      <c r="B72" s="28"/>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="26"/>
-      <c r="B73" s="27"/>
+      <c r="A73" s="27"/>
+      <c r="B73" s="28"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="26"/>
-      <c r="B74" s="27"/>
+      <c r="A74" s="27"/>
+      <c r="B74" s="28"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="26"/>
-      <c r="B75" s="27"/>
+      <c r="A75" s="27"/>
+      <c r="B75" s="28"/>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="26"/>
-      <c r="B76" s="27"/>
+      <c r="A76" s="27"/>
+      <c r="B76" s="28"/>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="26"/>
-      <c r="B77" s="27"/>
+      <c r="A77" s="27"/>
+      <c r="B77" s="28"/>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="26"/>
-      <c r="B78" s="27"/>
+      <c r="A78" s="27"/>
+      <c r="B78" s="28"/>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="26"/>
-      <c r="B79" s="27"/>
+      <c r="A79" s="27"/>
+      <c r="B79" s="28"/>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="26"/>
-      <c r="B80" s="27"/>
+      <c r="A80" s="27"/>
+      <c r="B80" s="28"/>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="26"/>
-      <c r="B81" s="27"/>
+      <c r="A81" s="27"/>
+      <c r="B81" s="28"/>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="26"/>
-      <c r="B82" s="27"/>
+      <c r="A82" s="27"/>
+      <c r="B82" s="28"/>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="26"/>
-      <c r="B83" s="27"/>
+      <c r="A83" s="27"/>
+      <c r="B83" s="28"/>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="26"/>
-      <c r="B84" s="27"/>
+      <c r="A84" s="27"/>
+      <c r="B84" s="28"/>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="26"/>
-      <c r="B85" s="27"/>
+      <c r="A85" s="27"/>
+      <c r="B85" s="28"/>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="26"/>
-      <c r="B86" s="27"/>
+      <c r="A86" s="27"/>
+      <c r="B86" s="28"/>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="26"/>
-      <c r="B87" s="27"/>
+      <c r="A87" s="27"/>
+      <c r="B87" s="28"/>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="26"/>
-      <c r="B88" s="27"/>
+      <c r="A88" s="27"/>
+      <c r="B88" s="28"/>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="26"/>
-      <c r="B89" s="27"/>
+      <c r="A89" s="27"/>
+      <c r="B89" s="28"/>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="26"/>
-      <c r="B90" s="27"/>
+      <c r="A90" s="27"/>
+      <c r="B90" s="28"/>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" s="26"/>
-      <c r="B91" s="27"/>
+      <c r="A91" s="27"/>
+      <c r="B91" s="28"/>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" s="26"/>
-      <c r="B92" s="27"/>
+      <c r="A92" s="27"/>
+      <c r="B92" s="28"/>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" s="26"/>
-      <c r="B93" s="27"/>
+      <c r="A93" s="27"/>
+      <c r="B93" s="28"/>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="26"/>
-      <c r="B94" s="27"/>
+      <c r="A94" s="27"/>
+      <c r="B94" s="28"/>
     </row>
     <row r="95" spans="1:2">
-      <c r="A95" s="26"/>
-      <c r="B95" s="27"/>
+      <c r="A95" s="27"/>
+      <c r="B95" s="28"/>
     </row>
     <row r="96" spans="1:2">
-      <c r="A96" s="26"/>
-      <c r="B96" s="27"/>
+      <c r="A96" s="27"/>
+      <c r="B96" s="28"/>
     </row>
     <row r="97" spans="1:2">
-      <c r="A97" s="26"/>
-      <c r="B97" s="27"/>
+      <c r="A97" s="27"/>
+      <c r="B97" s="28"/>
     </row>
     <row r="98" spans="1:2">
-      <c r="A98" s="26"/>
-      <c r="B98" s="27"/>
+      <c r="A98" s="27"/>
+      <c r="B98" s="28"/>
     </row>
     <row r="99" spans="1:2">
-      <c r="A99" s="26"/>
-      <c r="B99" s="27"/>
+      <c r="A99" s="27"/>
+      <c r="B99" s="28"/>
     </row>
     <row r="100" spans="1:2">
-      <c r="A100" s="26"/>
-      <c r="B100" s="27"/>
+      <c r="A100" s="27"/>
+      <c r="B100" s="28"/>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="26"/>
-      <c r="B101" s="27"/>
+      <c r="A101" s="27"/>
+      <c r="B101" s="28"/>
     </row>
     <row r="102" spans="1:2">
-      <c r="A102" s="26"/>
-      <c r="B102" s="27"/>
+      <c r="A102" s="27"/>
+      <c r="B102" s="28"/>
     </row>
     <row r="103" spans="1:2">
-      <c r="A103" s="26"/>
-      <c r="B103" s="27"/>
+      <c r="A103" s="27"/>
+      <c r="B103" s="28"/>
     </row>
     <row r="104" spans="1:2">
-      <c r="A104" s="26"/>
-      <c r="B104" s="27"/>
+      <c r="A104" s="27"/>
+      <c r="B104" s="28"/>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" s="26"/>
-      <c r="B105" s="27"/>
+      <c r="A105" s="27"/>
+      <c r="B105" s="28"/>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" s="26"/>
-      <c r="B106" s="27"/>
+      <c r="A106" s="27"/>
+      <c r="B106" s="28"/>
     </row>
     <row r="107" spans="1:2">
-      <c r="A107" s="26"/>
-      <c r="B107" s="27"/>
+      <c r="A107" s="27"/>
+      <c r="B107" s="28"/>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="26"/>
-      <c r="B108" s="27"/>
+      <c r="A108" s="27"/>
+      <c r="B108" s="28"/>
     </row>
     <row r="109" spans="1:2">
-      <c r="A109" s="26"/>
-      <c r="B109" s="27"/>
+      <c r="A109" s="27"/>
+      <c r="B109" s="28"/>
     </row>
     <row r="110" spans="1:2">
-      <c r="A110" s="26"/>
-      <c r="B110" s="27"/>
+      <c r="A110" s="27"/>
+      <c r="B110" s="28"/>
     </row>
     <row r="111" spans="1:2">
-      <c r="A111" s="26"/>
-      <c r="B111" s="27"/>
+      <c r="A111" s="27"/>
+      <c r="B111" s="28"/>
     </row>
     <row r="112" spans="1:2">
-      <c r="A112" s="26"/>
-      <c r="B112" s="27"/>
+      <c r="A112" s="27"/>
+      <c r="B112" s="28"/>
     </row>
     <row r="113" spans="1:2">
-      <c r="A113" s="26"/>
-      <c r="B113" s="27"/>
+      <c r="A113" s="27"/>
+      <c r="B113" s="28"/>
     </row>
     <row r="114" spans="1:2">
-      <c r="A114" s="26"/>
-      <c r="B114" s="27"/>
+      <c r="A114" s="27"/>
+      <c r="B114" s="28"/>
     </row>
     <row r="115" spans="1:2">
-      <c r="A115" s="26"/>
-      <c r="B115" s="27"/>
+      <c r="A115" s="27"/>
+      <c r="B115" s="28"/>
     </row>
     <row r="116" spans="1:2">
-      <c r="A116" s="26"/>
-      <c r="B116" s="27"/>
+      <c r="A116" s="27"/>
+      <c r="B116" s="28"/>
     </row>
     <row r="117" spans="1:2">
-      <c r="A117" s="26"/>
-      <c r="B117" s="27"/>
+      <c r="A117" s="27"/>
+      <c r="B117" s="28"/>
     </row>
     <row r="118" spans="1:2">
-      <c r="A118" s="26"/>
-      <c r="B118" s="27"/>
+      <c r="A118" s="27"/>
+      <c r="B118" s="28"/>
     </row>
     <row r="119" spans="1:2">
-      <c r="A119" s="26"/>
-      <c r="B119" s="27"/>
+      <c r="A119" s="27"/>
+      <c r="B119" s="28"/>
     </row>
     <row r="120" spans="1:2">
-      <c r="A120" s="26"/>
-      <c r="B120" s="27"/>
+      <c r="A120" s="27"/>
+      <c r="B120" s="28"/>
     </row>
     <row r="121" spans="1:2">
-      <c r="A121" s="26"/>
-      <c r="B121" s="27"/>
+      <c r="A121" s="27"/>
+      <c r="B121" s="28"/>
     </row>
     <row r="122" spans="1:2">
-      <c r="A122" s="26"/>
-      <c r="B122" s="27"/>
+      <c r="A122" s="27"/>
+      <c r="B122" s="28"/>
     </row>
     <row r="123" spans="1:2">
-      <c r="A123" s="26"/>
-      <c r="B123" s="27"/>
+      <c r="A123" s="27"/>
+      <c r="B123" s="28"/>
     </row>
     <row r="124" spans="1:2">
-      <c r="A124" s="26"/>
-      <c r="B124" s="27"/>
+      <c r="A124" s="27"/>
+      <c r="B124" s="28"/>
     </row>
     <row r="125" spans="1:2">
-      <c r="A125" s="26"/>
-      <c r="B125" s="27"/>
+      <c r="A125" s="27"/>
+      <c r="B125" s="28"/>
     </row>
     <row r="126" spans="1:2">
-      <c r="A126" s="26"/>
-      <c r="B126" s="27"/>
+      <c r="A126" s="27"/>
+      <c r="B126" s="28"/>
     </row>
     <row r="127" spans="1:2">
-      <c r="A127" s="26"/>
-      <c r="B127" s="27"/>
+      <c r="A127" s="27"/>
+      <c r="B127" s="28"/>
     </row>
     <row r="128" spans="1:2">
-      <c r="A128" s="26"/>
-      <c r="B128" s="27"/>
+      <c r="A128" s="27"/>
+      <c r="B128" s="28"/>
     </row>
     <row r="129" spans="1:2">
-      <c r="A129" s="26"/>
-      <c r="B129" s="27"/>
+      <c r="A129" s="27"/>
+      <c r="B129" s="28"/>
     </row>
     <row r="130" spans="1:2">
-      <c r="A130" s="26"/>
-      <c r="B130" s="27"/>
+      <c r="A130" s="27"/>
+      <c r="B130" s="28"/>
     </row>
     <row r="131" spans="1:2">
-      <c r="A131" s="26"/>
-      <c r="B131" s="27"/>
+      <c r="A131" s="27"/>
+      <c r="B131" s="28"/>
     </row>
     <row r="132" spans="1:2">
-      <c r="A132" s="26"/>
-      <c r="B132" s="27"/>
+      <c r="A132" s="27"/>
+      <c r="B132" s="28"/>
     </row>
     <row r="133" spans="1:2">
-      <c r="A133" s="26"/>
-      <c r="B133" s="27"/>
+      <c r="A133" s="27"/>
+      <c r="B133" s="28"/>
     </row>
     <row r="134" spans="1:2">
-      <c r="A134" s="26"/>
-      <c r="B134" s="27"/>
+      <c r="A134" s="27"/>
+      <c r="B134" s="28"/>
     </row>
     <row r="135" spans="1:2">
-      <c r="A135" s="26"/>
-      <c r="B135" s="27"/>
+      <c r="A135" s="27"/>
+      <c r="B135" s="28"/>
     </row>
     <row r="136" spans="1:2">
-      <c r="A136" s="26"/>
-      <c r="B136" s="27"/>
+      <c r="A136" s="27"/>
+      <c r="B136" s="28"/>
     </row>
     <row r="137" spans="1:2">
-      <c r="A137" s="26"/>
-      <c r="B137" s="27"/>
+      <c r="A137" s="27"/>
+      <c r="B137" s="28"/>
     </row>
     <row r="138" spans="1:2">
-      <c r="A138" s="26"/>
-      <c r="B138" s="27"/>
+      <c r="A138" s="27"/>
+      <c r="B138" s="28"/>
     </row>
     <row r="139" spans="1:2">
-      <c r="A139" s="26"/>
-      <c r="B139" s="27"/>
+      <c r="A139" s="27"/>
+      <c r="B139" s="28"/>
     </row>
     <row r="140" spans="1:2">
-      <c r="A140" s="26"/>
-      <c r="B140" s="27"/>
+      <c r="A140" s="27"/>
+      <c r="B140" s="28"/>
     </row>
     <row r="141" spans="1:2">
-      <c r="A141" s="26"/>
-      <c r="B141" s="27"/>
+      <c r="A141" s="27"/>
+      <c r="B141" s="28"/>
     </row>
     <row r="142" spans="1:2">
-      <c r="A142" s="26"/>
-      <c r="B142" s="27"/>
+      <c r="A142" s="27"/>
+      <c r="B142" s="28"/>
     </row>
     <row r="143" spans="1:2">
-      <c r="A143" s="26"/>
-      <c r="B143" s="27"/>
+      <c r="A143" s="27"/>
+      <c r="B143" s="28"/>
     </row>
     <row r="144" spans="1:2">
-      <c r="A144" s="26"/>
-      <c r="B144" s="27"/>
+      <c r="A144" s="27"/>
+      <c r="B144" s="28"/>
     </row>
     <row r="145" spans="1:2">
-      <c r="A145" s="26"/>
-      <c r="B145" s="27"/>
+      <c r="A145" s="27"/>
+      <c r="B145" s="28"/>
     </row>
     <row r="146" spans="1:2">
-      <c r="A146" s="26"/>
-      <c r="B146" s="27"/>
+      <c r="A146" s="27"/>
+      <c r="B146" s="28"/>
     </row>
     <row r="147" spans="1:2">
-      <c r="A147" s="26"/>
-      <c r="B147" s="27"/>
+      <c r="A147" s="27"/>
+      <c r="B147" s="28"/>
     </row>
     <row r="148" spans="1:2">
-      <c r="A148" s="26"/>
-      <c r="B148" s="27"/>
+      <c r="A148" s="27"/>
+      <c r="B148" s="28"/>
     </row>
     <row r="149" spans="1:2">
-      <c r="A149" s="26"/>
-      <c r="B149" s="27"/>
+      <c r="A149" s="27"/>
+      <c r="B149" s="28"/>
     </row>
     <row r="150" spans="1:2">
-      <c r="A150" s="26"/>
-      <c r="B150" s="27"/>
+      <c r="A150" s="27"/>
+      <c r="B150" s="28"/>
     </row>
     <row r="151" spans="1:2">
-      <c r="A151" s="26"/>
-      <c r="B151" s="27"/>
+      <c r="A151" s="27"/>
+      <c r="B151" s="28"/>
     </row>
     <row r="152" spans="1:2">
-      <c r="A152" s="26"/>
-      <c r="B152" s="27"/>
+      <c r="A152" s="27"/>
+      <c r="B152" s="28"/>
     </row>
     <row r="153" spans="1:2">
-      <c r="A153" s="26"/>
-      <c r="B153" s="27"/>
+      <c r="A153" s="27"/>
+      <c r="B153" s="28"/>
     </row>
     <row r="154" spans="1:2">
-      <c r="A154" s="26"/>
-      <c r="B154" s="27"/>
+      <c r="A154" s="27"/>
+      <c r="B154" s="28"/>
     </row>
     <row r="155" spans="1:2">
-      <c r="A155" s="26"/>
-      <c r="B155" s="27"/>
+      <c r="A155" s="27"/>
+      <c r="B155" s="28"/>
     </row>
     <row r="156" spans="1:2">
-      <c r="A156" s="26"/>
-      <c r="B156" s="27"/>
+      <c r="A156" s="27"/>
+      <c r="B156" s="28"/>
     </row>
     <row r="157" spans="1:2">
-      <c r="A157" s="26"/>
-      <c r="B157" s="27"/>
+      <c r="A157" s="27"/>
+      <c r="B157" s="28"/>
     </row>
     <row r="158" spans="1:2">
-      <c r="A158" s="26"/>
-      <c r="B158" s="27"/>
+      <c r="A158" s="27"/>
+      <c r="B158" s="28"/>
     </row>
     <row r="159" spans="1:2">
-      <c r="A159" s="26"/>
-      <c r="B159" s="27"/>
+      <c r="A159" s="27"/>
+      <c r="B159" s="28"/>
     </row>
     <row r="160" spans="1:2">
-      <c r="A160" s="26"/>
-      <c r="B160" s="27"/>
+      <c r="A160" s="27"/>
+      <c r="B160" s="28"/>
     </row>
     <row r="161" spans="1:2">
-      <c r="A161" s="26"/>
-      <c r="B161" s="27"/>
+      <c r="A161" s="27"/>
+      <c r="B161" s="28"/>
     </row>
     <row r="162" spans="1:2">
-      <c r="A162" s="26"/>
-      <c r="B162" s="27"/>
+      <c r="A162" s="27"/>
+      <c r="B162" s="28"/>
     </row>
     <row r="163" spans="1:2">
-      <c r="A163" s="26"/>
-      <c r="B163" s="27"/>
+      <c r="A163" s="27"/>
+      <c r="B163" s="28"/>
     </row>
     <row r="164" spans="1:2">
-      <c r="A164" s="26"/>
-      <c r="B164" s="27"/>
+      <c r="A164" s="27"/>
+      <c r="B164" s="28"/>
     </row>
     <row r="165" spans="1:2">
-      <c r="A165" s="26"/>
-      <c r="B165" s="27"/>
+      <c r="A165" s="27"/>
+      <c r="B165" s="28"/>
     </row>
     <row r="166" spans="1:2">
-      <c r="A166" s="26"/>
-      <c r="B166" s="27"/>
+      <c r="A166" s="27"/>
+      <c r="B166" s="28"/>
     </row>
     <row r="167" spans="1:2">
-      <c r="A167" s="26"/>
-      <c r="B167" s="27"/>
+      <c r="A167" s="27"/>
+      <c r="B167" s="28"/>
     </row>
     <row r="168" spans="1:2">
-      <c r="A168" s="26"/>
-      <c r="B168" s="27"/>
+      <c r="A168" s="27"/>
+      <c r="B168" s="28"/>
     </row>
     <row r="169" spans="1:2">
-      <c r="A169" s="26"/>
-      <c r="B169" s="27"/>
+      <c r="A169" s="27"/>
+      <c r="B169" s="28"/>
     </row>
     <row r="170" spans="1:2">
-      <c r="A170" s="26"/>
-      <c r="B170" s="27"/>
+      <c r="A170" s="27"/>
+      <c r="B170" s="28"/>
     </row>
     <row r="171" spans="1:2">
-      <c r="A171" s="26"/>
-      <c r="B171" s="27"/>
+      <c r="A171" s="27"/>
+      <c r="B171" s="28"/>
     </row>
     <row r="172" spans="1:2">
-      <c r="A172" s="26"/>
-      <c r="B172" s="27"/>
+      <c r="A172" s="27"/>
+      <c r="B172" s="28"/>
     </row>
     <row r="173" spans="1:2">
-      <c r="A173" s="26"/>
-      <c r="B173" s="27"/>
+      <c r="A173" s="27"/>
+      <c r="B173" s="28"/>
     </row>
     <row r="174" spans="1:2">
-      <c r="A174" s="26"/>
-      <c r="B174" s="27"/>
+      <c r="A174" s="27"/>
+      <c r="B174" s="28"/>
     </row>
     <row r="175" spans="1:2">
-      <c r="A175" s="26"/>
-      <c r="B175" s="27"/>
+      <c r="A175" s="27"/>
+      <c r="B175" s="28"/>
     </row>
     <row r="176" spans="1:2">
-      <c r="A176" s="26"/>
-      <c r="B176" s="27"/>
+      <c r="A176" s="27"/>
+      <c r="B176" s="28"/>
     </row>
     <row r="177" spans="1:2">
-      <c r="A177" s="26"/>
-      <c r="B177" s="27"/>
+      <c r="A177" s="27"/>
+      <c r="B177" s="28"/>
     </row>
     <row r="178" spans="1:2">
-      <c r="A178" s="26"/>
-      <c r="B178" s="27"/>
+      <c r="A178" s="27"/>
+      <c r="B178" s="28"/>
     </row>
     <row r="179" spans="1:2">
-      <c r="A179" s="26"/>
-      <c r="B179" s="27"/>
+      <c r="A179" s="27"/>
+      <c r="B179" s="28"/>
     </row>
     <row r="180" spans="1:2">
-      <c r="A180" s="26"/>
-      <c r="B180" s="27"/>
+      <c r="A180" s="27"/>
+      <c r="B180" s="28"/>
     </row>
     <row r="181" spans="1:2">
-      <c r="A181" s="26"/>
-      <c r="B181" s="27"/>
+      <c r="A181" s="27"/>
+      <c r="B181" s="28"/>
     </row>
     <row r="182" spans="1:2">
-      <c r="A182" s="26"/>
-      <c r="B182" s="27"/>
+      <c r="A182" s="27"/>
+      <c r="B182" s="28"/>
     </row>
     <row r="183" spans="1:2">
-      <c r="A183" s="26"/>
-      <c r="B183" s="27"/>
+      <c r="A183" s="27"/>
+      <c r="B183" s="28"/>
     </row>
     <row r="184" spans="1:2">
-      <c r="A184" s="26"/>
-      <c r="B184" s="27"/>
+      <c r="A184" s="27"/>
+      <c r="B184" s="28"/>
     </row>
     <row r="185" spans="1:2">
-      <c r="A185" s="26"/>
-      <c r="B185" s="27"/>
+      <c r="A185" s="27"/>
+      <c r="B185" s="28"/>
     </row>
     <row r="186" spans="1:2">
-      <c r="A186" s="26"/>
-      <c r="B186" s="27"/>
+      <c r="A186" s="27"/>
+      <c r="B186" s="28"/>
     </row>
     <row r="187" spans="1:2">
-      <c r="A187" s="26"/>
-      <c r="B187" s="27"/>
+      <c r="A187" s="27"/>
+      <c r="B187" s="28"/>
     </row>
     <row r="188" spans="1:2">
-      <c r="A188" s="26"/>
-      <c r="B188" s="27"/>
+      <c r="A188" s="27"/>
+      <c r="B188" s="28"/>
     </row>
     <row r="189" spans="1:2">
-      <c r="A189" s="26"/>
-      <c r="B189" s="27"/>
+      <c r="A189" s="27"/>
+      <c r="B189" s="28"/>
     </row>
     <row r="190" spans="1:2">
-      <c r="A190" s="26"/>
-      <c r="B190" s="27"/>
+      <c r="A190" s="27"/>
+      <c r="B190" s="28"/>
     </row>
     <row r="191" spans="1:2">
-      <c r="A191" s="26"/>
-      <c r="B191" s="27"/>
+      <c r="A191" s="27"/>
+      <c r="B191" s="28"/>
     </row>
     <row r="192" spans="1:2">
-      <c r="A192" s="26"/>
-      <c r="B192" s="27"/>
+      <c r="A192" s="27"/>
+      <c r="B192" s="28"/>
     </row>
     <row r="193" spans="1:2">
-      <c r="A193" s="26"/>
-      <c r="B193" s="27"/>
+      <c r="A193" s="27"/>
+      <c r="B193" s="28"/>
     </row>
     <row r="194" spans="1:2">
-      <c r="A194" s="26"/>
-      <c r="B194" s="27"/>
+      <c r="A194" s="27"/>
+      <c r="B194" s="28"/>
     </row>
     <row r="195" spans="1:2">
-      <c r="A195" s="26"/>
-      <c r="B195" s="27"/>
+      <c r="A195" s="27"/>
+      <c r="B195" s="28"/>
     </row>
     <row r="196" spans="1:2">
-      <c r="A196" s="26"/>
-      <c r="B196" s="27"/>
+      <c r="A196" s="27"/>
+      <c r="B196" s="28"/>
     </row>
     <row r="197" spans="1:2">
-      <c r="A197" s="26"/>
-      <c r="B197" s="27"/>
+      <c r="A197" s="27"/>
+      <c r="B197" s="28"/>
     </row>
     <row r="198" spans="1:2">
-      <c r="A198" s="26"/>
-      <c r="B198" s="27"/>
+      <c r="A198" s="27"/>
+      <c r="B198" s="28"/>
     </row>
     <row r="199" spans="1:2">
-      <c r="A199" s="26"/>
-      <c r="B199" s="27"/>
+      <c r="A199" s="27"/>
+      <c r="B199" s="28"/>
     </row>
     <row r="200" spans="1:2">
-      <c r="A200" s="26"/>
-      <c r="B200" s="27"/>
+      <c r="A200" s="27"/>
+      <c r="B200" s="28"/>
     </row>
     <row r="201" spans="1:2">
-      <c r="A201" s="26"/>
-      <c r="B201" s="27"/>
+      <c r="A201" s="27"/>
+      <c r="B201" s="28"/>
     </row>
     <row r="202" spans="1:2">
-      <c r="A202" s="26"/>
-      <c r="B202" s="27"/>
+      <c r="A202" s="27"/>
+      <c r="B202" s="28"/>
     </row>
     <row r="203" spans="1:2">
-      <c r="A203" s="26"/>
-      <c r="B203" s="27"/>
+      <c r="A203" s="27"/>
+      <c r="B203" s="28"/>
     </row>
     <row r="204" spans="1:2">
-      <c r="A204" s="26"/>
-      <c r="B204" s="27"/>
+      <c r="A204" s="27"/>
+      <c r="B204" s="28"/>
     </row>
     <row r="205" spans="1:2">
-      <c r="A205" s="26"/>
-      <c r="B205" s="27"/>
+      <c r="A205" s="27"/>
+      <c r="B205" s="28"/>
     </row>
     <row r="206" spans="1:2">
-      <c r="A206" s="26"/>
-      <c r="B206" s="27"/>
+      <c r="A206" s="27"/>
+      <c r="B206" s="28"/>
     </row>
     <row r="207" spans="1:2">
-      <c r="A207" s="26"/>
-      <c r="B207" s="27"/>
+      <c r="A207" s="27"/>
+      <c r="B207" s="28"/>
     </row>
     <row r="208" spans="1:2">
-      <c r="A208" s="26"/>
-      <c r="B208" s="27"/>
+      <c r="A208" s="27"/>
+      <c r="B208" s="28"/>
     </row>
     <row r="209" spans="1:2">
-      <c r="A209" s="26"/>
-      <c r="B209" s="27"/>
+      <c r="A209" s="27"/>
+      <c r="B209" s="28"/>
     </row>
     <row r="210" spans="1:2">
-      <c r="A210" s="26"/>
-      <c r="B210" s="27"/>
+      <c r="A210" s="27"/>
+      <c r="B210" s="28"/>
     </row>
     <row r="211" spans="1:2">
-      <c r="A211" s="26"/>
-      <c r="B211" s="27"/>
+      <c r="A211" s="27"/>
+      <c r="B211" s="28"/>
     </row>
     <row r="212" spans="1:2">
-      <c r="A212" s="26"/>
-      <c r="B212" s="27"/>
+      <c r="A212" s="27"/>
+      <c r="B212" s="28"/>
     </row>
     <row r="213" spans="1:2">
-      <c r="A213" s="26"/>
-      <c r="B213" s="27"/>
+      <c r="A213" s="27"/>
+      <c r="B213" s="28"/>
     </row>
     <row r="214" spans="1:2">
-      <c r="A214" s="26"/>
-      <c r="B214" s="27"/>
+      <c r="A214" s="27"/>
+      <c r="B214" s="28"/>
     </row>
     <row r="215" spans="1:2">
-      <c r="A215" s="26"/>
-      <c r="B215" s="27"/>
+      <c r="A215" s="27"/>
+      <c r="B215" s="28"/>
     </row>
     <row r="216" spans="1:2">
-      <c r="A216" s="26"/>
-      <c r="B216" s="27"/>
+      <c r="A216" s="27"/>
+      <c r="B216" s="28"/>
     </row>
     <row r="217" spans="1:2">
-      <c r="A217" s="26"/>
-      <c r="B217" s="27"/>
+      <c r="A217" s="27"/>
+      <c r="B217" s="28"/>
     </row>
     <row r="218" spans="1:2">
-      <c r="A218" s="26"/>
-      <c r="B218" s="27"/>
+      <c r="A218" s="27"/>
+      <c r="B218" s="28"/>
     </row>
     <row r="219" spans="1:2">
-      <c r="A219" s="26"/>
-      <c r="B219" s="27"/>
+      <c r="A219" s="27"/>
+      <c r="B219" s="28"/>
     </row>
     <row r="220" spans="1:2">
-      <c r="A220" s="26"/>
-      <c r="B220" s="27"/>
+      <c r="A220" s="27"/>
+      <c r="B220" s="28"/>
     </row>
     <row r="221" spans="1:2">
-      <c r="A221" s="26"/>
-      <c r="B221" s="27"/>
+      <c r="A221" s="27"/>
+      <c r="B221" s="28"/>
     </row>
     <row r="222" spans="1:2">
-      <c r="A222" s="26"/>
-      <c r="B222" s="27"/>
+      <c r="A222" s="27"/>
+      <c r="B222" s="28"/>
     </row>
     <row r="223" spans="1:2">
-      <c r="A223" s="26"/>
-      <c r="B223" s="27"/>
+      <c r="A223" s="27"/>
+      <c r="B223" s="28"/>
     </row>
     <row r="224" spans="1:2">
-      <c r="A224" s="26"/>
-      <c r="B224" s="27"/>
+      <c r="A224" s="27"/>
+      <c r="B224" s="28"/>
     </row>
     <row r="225" spans="1:2">
-      <c r="A225" s="26"/>
-      <c r="B225" s="27"/>
+      <c r="A225" s="27"/>
+      <c r="B225" s="28"/>
     </row>
     <row r="226" spans="1:2">
-      <c r="A226" s="26"/>
-      <c r="B226" s="27"/>
+      <c r="A226" s="27"/>
+      <c r="B226" s="28"/>
     </row>
     <row r="227" spans="1:2">
-      <c r="A227" s="26"/>
-      <c r="B227" s="27"/>
+      <c r="A227" s="27"/>
+      <c r="B227" s="28"/>
     </row>
     <row r="228" spans="1:2">
-      <c r="A228" s="26"/>
-      <c r="B228" s="27"/>
+      <c r="A228" s="27"/>
+      <c r="B228" s="28"/>
     </row>
     <row r="229" spans="1:2">
-      <c r="A229" s="26"/>
-      <c r="B229" s="27"/>
+      <c r="A229" s="27"/>
+      <c r="B229" s="28"/>
     </row>
     <row r="230" spans="1:2">
-      <c r="A230" s="26"/>
-      <c r="B230" s="27"/>
+      <c r="A230" s="27"/>
+      <c r="B230" s="28"/>
     </row>
     <row r="231" spans="1:2">
-      <c r="A231" s="26"/>
-      <c r="B231" s="27"/>
+      <c r="A231" s="27"/>
+      <c r="B231" s="28"/>
     </row>
     <row r="232" spans="1:2">
-      <c r="A232" s="26"/>
-      <c r="B232" s="27"/>
+      <c r="A232" s="27"/>
+      <c r="B232" s="28"/>
     </row>
     <row r="233" spans="1:2">
-      <c r="A233" s="26"/>
-      <c r="B233" s="27"/>
+      <c r="A233" s="27"/>
+      <c r="B233" s="28"/>
     </row>
     <row r="234" spans="1:2">
-      <c r="A234" s="26"/>
-      <c r="B234" s="27"/>
+      <c r="A234" s="27"/>
+      <c r="B234" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -5668,72 +5750,72 @@
       <c r="E1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="31"/>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="31"/>
-      <c r="BH1" s="31"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="31"/>
-      <c r="BM1" s="31"/>
-      <c r="BN1" s="31"/>
-      <c r="BO1" s="31"/>
-      <c r="BP1" s="31"/>
-      <c r="BQ1" s="31"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="32"/>
+      <c r="BH1" s="32"/>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BM1" s="32"/>
+      <c r="BN1" s="32"/>
+      <c r="BO1" s="32"/>
+      <c r="BP1" s="32"/>
+      <c r="BQ1" s="32"/>
     </row>
     <row r="2" spans="1:69">
       <c r="A2" s="4" t="s">
@@ -6049,13 +6131,13 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6074,15 +6156,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BP39"/>
+  <dimension ref="A1:BP49"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="69.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="23.6640625" style="8" customWidth="1"/>
     <col min="4" max="4" width="26" style="3" customWidth="1"/>
@@ -6093,7 +6175,7 @@
   <sheetData>
     <row r="1" spans="1:68">
       <c r="A1" s="3" t="s">
-        <v>108</v>
+        <v>219</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>44</v>
@@ -6104,72 +6186,72 @@
       <c r="D1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="31"/>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="31"/>
-      <c r="BH1" s="31"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="31"/>
-      <c r="BM1" s="31"/>
-      <c r="BN1" s="31"/>
-      <c r="BO1" s="31"/>
-      <c r="BP1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="32"/>
+      <c r="BH1" s="32"/>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BM1" s="32"/>
+      <c r="BN1" s="32"/>
+      <c r="BO1" s="32"/>
+      <c r="BP1" s="32"/>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="9" t="s">
@@ -6181,13 +6263,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:68">
@@ -6196,13 +6278,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:68">
@@ -6211,13 +6293,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:68">
@@ -6226,10 +6308,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>88</v>
@@ -6241,13 +6323,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:68">
@@ -6256,13 +6338,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:68">
@@ -6271,13 +6353,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:68">
@@ -6286,13 +6368,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:68">
@@ -6301,10 +6383,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>88</v>
@@ -6316,13 +6398,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:68">
@@ -6339,12 +6421,12 @@
     </row>
     <row r="15" spans="1:68">
       <c r="B15" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>122</v>
+        <v>218</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>44</v>
@@ -6366,13 +6448,13 @@
         <v>0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -6381,13 +6463,13 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -6396,13 +6478,13 @@
         <v>2</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -6411,10 +6493,10 @@
         <v>3</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>88</v>
@@ -6426,13 +6508,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -6441,13 +6523,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -6456,13 +6538,13 @@
         <v>6</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -6471,10 +6553,10 @@
         <v>7</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>88</v>
@@ -6486,13 +6568,13 @@
         <v>8</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -6501,13 +6583,13 @@
         <v>9</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -6516,13 +6598,13 @@
         <v>10</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -6531,13 +6613,13 @@
         <v>11</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -6546,10 +6628,10 @@
         <v>12</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>88</v>
@@ -6561,13 +6643,13 @@
         <v>13</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -6576,13 +6658,13 @@
         <v>14</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -6591,13 +6673,13 @@
         <v>15</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -6606,10 +6688,10 @@
         <v>16</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>88</v>
@@ -6621,13 +6703,13 @@
         <v>17</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -6644,14 +6726,81 @@
     </row>
     <row r="39" spans="1:4">
       <c r="B39" s="3" t="s">
-        <v>131</v>
-      </c>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="3">
+        <v>0</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="D44" s="33" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="3">
+        <f>A44+1</f>
+        <v>1</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D45" s="34" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="3">
+        <f t="shared" ref="A46:A54" si="1">A45+1</f>
+        <v>2</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="8">
+        <v>25</v>
+      </c>
+      <c r="D46" s="34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4">
+      <c r="D49" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E1:BP1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6692,72 +6841,72 @@
       <c r="D1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="31"/>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="31"/>
-      <c r="BH1" s="31"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="31"/>
-      <c r="BM1" s="31"/>
-      <c r="BN1" s="31"/>
-      <c r="BO1" s="31"/>
-      <c r="BP1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="32"/>
+      <c r="BH1" s="32"/>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BM1" s="32"/>
+      <c r="BN1" s="32"/>
+      <c r="BO1" s="32"/>
+      <c r="BP1" s="32"/>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="9" t="s">
@@ -6769,13 +6918,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:68">
@@ -6784,13 +6933,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:68">
@@ -6799,13 +6948,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:68">
@@ -6814,10 +6963,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>88</v>
@@ -6829,13 +6978,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>140</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:68">
@@ -6844,13 +6993,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:68">
@@ -6859,13 +7008,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:68">
@@ -6882,14 +7031,14 @@
     </row>
     <row r="25" spans="1:4">
       <c r="B25" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6937,72 +7086,72 @@
       <c r="D1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="31"/>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="31"/>
-      <c r="BH1" s="31"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="31"/>
-      <c r="BM1" s="31"/>
-      <c r="BN1" s="31"/>
-      <c r="BO1" s="31"/>
-      <c r="BP1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="32"/>
+      <c r="BH1" s="32"/>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BM1" s="32"/>
+      <c r="BN1" s="32"/>
+      <c r="BO1" s="32"/>
+      <c r="BP1" s="32"/>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="9" t="s">
@@ -7014,13 +7163,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:68">
@@ -7029,13 +7178,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>150</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:68">
@@ -7044,13 +7193,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>150</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:68">
@@ -7059,10 +7208,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>88</v>
@@ -7074,13 +7223,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>140</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:68">
@@ -7089,13 +7238,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:68">
@@ -7104,13 +7253,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:68">
@@ -7127,14 +7276,14 @@
     </row>
     <row r="25" spans="1:4">
       <c r="B25" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7182,72 +7331,72 @@
       <c r="D1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="31"/>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="31"/>
-      <c r="BH1" s="31"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="31"/>
-      <c r="BM1" s="31"/>
-      <c r="BN1" s="31"/>
-      <c r="BO1" s="31"/>
-      <c r="BP1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="32"/>
+      <c r="BH1" s="32"/>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BM1" s="32"/>
+      <c r="BN1" s="32"/>
+      <c r="BO1" s="32"/>
+      <c r="BP1" s="32"/>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="10" t="s">
@@ -7262,13 +7411,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:68">
@@ -7277,13 +7426,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:68">
@@ -7292,13 +7441,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:68">
@@ -7306,10 +7455,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>88</v>
@@ -7320,13 +7469,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:68">
@@ -7340,19 +7489,19 @@
         <v>26</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:68">
       <c r="B11" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7385,7 +7534,7 @@
   <sheetData>
     <row r="1" spans="1:68" ht="15">
       <c r="A1" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>44</v>
@@ -7396,72 +7545,72 @@
       <c r="D1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="31"/>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="31"/>
-      <c r="BH1" s="31"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="31"/>
-      <c r="BM1" s="31"/>
-      <c r="BN1" s="31"/>
-      <c r="BO1" s="31"/>
-      <c r="BP1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="32"/>
+      <c r="BH1" s="32"/>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BM1" s="32"/>
+      <c r="BN1" s="32"/>
+      <c r="BO1" s="32"/>
+      <c r="BP1" s="32"/>
     </row>
     <row r="2" spans="1:68" ht="15">
       <c r="A2" s="10" t="s">
@@ -7540,13 +7689,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -7619,13 +7768,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -7698,13 +7847,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -7776,10 +7925,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>88</v>
@@ -7854,13 +8003,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -7938,7 +8087,7 @@
         <v>25</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -8037,7 +8186,7 @@
   <sheetData>
     <row r="1" spans="1:68">
       <c r="A1" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>44</v>
@@ -8048,72 +8197,72 @@
       <c r="D1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="31"/>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="31"/>
-      <c r="BH1" s="31"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="31"/>
-      <c r="BM1" s="31"/>
-      <c r="BN1" s="31"/>
-      <c r="BO1" s="31"/>
-      <c r="BP1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="32"/>
+      <c r="BH1" s="32"/>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BM1" s="32"/>
+      <c r="BN1" s="32"/>
+      <c r="BO1" s="32"/>
+      <c r="BP1" s="32"/>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="10" t="s">
@@ -8128,13 +8277,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:68">
@@ -8143,13 +8292,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:68">
@@ -8158,13 +8307,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:68">
@@ -8172,13 +8321,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:68">
@@ -8186,13 +8335,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:68">
@@ -8200,13 +8349,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:68">
@@ -8214,13 +8363,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:68">
@@ -8228,13 +8377,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:68">
@@ -8248,12 +8397,12 @@
         <v>25</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:68">
       <c r="B15" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>